<commit_message>
+version 2 + proyect chartery y WBS
</commit_message>
<xml_diff>
--- a/requisitos/Lista de Requerimientos-GCS.xlsx
+++ b/requisitos/Lista de Requerimientos-GCS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Código</t>
   </si>
@@ -54,12 +54,6 @@
     <t>toma de asistenacia</t>
   </si>
   <si>
-    <t>filtro de cola de tareas</t>
-  </si>
-  <si>
-    <t>monitoreo de una tarea</t>
-  </si>
-  <si>
     <t>Monitorear a travez de graficas las estadisticas d elas diferentes tareas</t>
   </si>
   <si>
@@ -69,33 +63,9 @@
     <t>culminar tarea</t>
   </si>
   <si>
-    <t>login</t>
-  </si>
-  <si>
     <t>recordar contraseña</t>
   </si>
   <si>
-    <t>poder mandar la contraseña al correo electronico</t>
-  </si>
-  <si>
-    <t>poder loguearse al sistema</t>
-  </si>
-  <si>
-    <t>mandar avisod e culminaciond e tarea</t>
-  </si>
-  <si>
-    <t>monitorear el avance de una tarea</t>
-  </si>
-  <si>
-    <t>filtrar las tareas según , tipo , usuario , estado</t>
-  </si>
-  <si>
-    <t>marcar asistencia</t>
-  </si>
-  <si>
-    <t>cambiar y rotar horarios</t>
-  </si>
-  <si>
     <t>crear y modificar cuentas de usuario</t>
   </si>
   <si>
@@ -132,64 +102,55 @@
     <t>Eysenck Gómez</t>
   </si>
   <si>
-    <t>Crear solicitud de tarea</t>
-  </si>
-  <si>
-    <t>Poder crear unma solicitud de tarea y que esta sea asginada inteligentemente al empleado mas capaz</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>Ver cola de tareas por cada empleado</t>
-  </si>
-  <si>
-    <t>Cada emplado podrá entrar al sistema y ver su cola de tareas para realizar</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>Ver cola de tareas general</t>
-  </si>
-  <si>
-    <t>Cada adminsitrador podrá ver la cola general de tareas y sus detalles</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>Filtrar tareas</t>
-  </si>
-  <si>
-    <t>Cada administrador podrá filtrar tareas por fecha, tipo, encargado.</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>Marcar tarea como realizada</t>
-  </si>
-  <si>
-    <t>El empleado podrá marcar la tarea como realizada.</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>Comentar tarea</t>
-  </si>
-  <si>
-    <t>Empleado y administrador podrán realizar comentarios sobre la tarea.</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>Aprobar comentario en tarea.</t>
-  </si>
-  <si>
-    <t>Los adminsitradores podrán aprobar los comentarios de los empleados para que sean visibles para todos.</t>
+    <t>José Ríos Vega</t>
+  </si>
+  <si>
+    <t>monitoreo</t>
+  </si>
+  <si>
+    <t>El sistema ofrecerá distintas gráficas para el monitoreo de las estadísticas de las distintas tareas.</t>
+  </si>
+  <si>
+    <t>filtrar de cola de tareas</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir a los administradores poder filtrar las tareas por categoria, tipo, fecha y empleado, mediante la elección del campo a filtrar.</t>
+  </si>
+  <si>
+    <t>mantenimiento de horarios</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir que el administrador pueda cambiar o rotar los horarios de cualquier empleado.</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir marcar asistencia a los empleados cuando estén dentro de sus horas, en otro caso no deber permitir el marcado de asistencia.</t>
+  </si>
+  <si>
+    <t>Kathy Velazquez</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir la creación y edición de usuarios por parte de los administradores.</t>
+  </si>
+  <si>
+    <t>loguearse al sistema</t>
+  </si>
+  <si>
+    <t>Elsistema debe permitir el logueo de 3 tipos de roles, administrador A, adminsitrador B, y empleado.</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir en caso de extravió de contraseña, hacer el cambio mediante un link al correo del usuario, para poder cambiar su contraseña.</t>
+  </si>
+  <si>
+    <t>mantenimiento de tareas</t>
+  </si>
+  <si>
+    <t>Solicitar crear tarea</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir que los administradores puedan solicitar la creaciñon de una tarea y que este la asigne a un empleado mediante un algoritmo.</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir que el usuario empleado pueda indicar el término de una tarea mediante un checkbox en la tarea.</t>
   </si>
 </sst>
 </file>
@@ -213,7 +174,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -236,11 +197,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,6 +233,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -553,20 +546,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G20"/>
+  <dimension ref="B3:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" customWidth="1"/>
-    <col min="7" max="7" width="63.42578125" customWidth="1"/>
+    <col min="7" max="7" width="135.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -600,12 +593,12 @@
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -614,12 +607,12 @@
         <v>8</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -628,218 +621,261 @@
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="F7" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>57</v>
-      </c>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>